<commit_message>
Recognize adductName column as non-sample column
[El-Maven v0.11.0 introduced a new output column,
`adductName`](https://github.com/ElucidataInc/ElMaven/releases/tag/v0.11.0).
TraceBase now recognizes this column and does not treat it as sample data.
Fixes #91.
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/small_dataset/small_obob_maven_6eaas_inf.xlsx
+++ b/DataRepo/example_data/small_dataset/small_obob_maven_6eaas_inf.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,105 +398,110 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>adductName</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>isotopeLabel</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>compound</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>compoundId</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>formula</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>expectedRtDiff</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>ppmDiff</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>parent</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>BAT-xz971</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Br-xz971</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Dia-xz971</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>gas-xz971</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>gWAT-xz971</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>H-xz971</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Kid-xz971</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Liv-xz971</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Lu-xz971</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Pc-xz971</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Q-xz971</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>SI-xz971</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Sol-xz971</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Sp-xz971</t>
         </is>
@@ -523,73 +528,78 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>C12 PARENT</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.5284548</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1.363487</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>179.0559</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>8814287</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>444513.3</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>5862178</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>6746356</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>10000000</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>8161388</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>26400000</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>37200000</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>10800000</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>6133946</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>8460165</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>15600000</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>2342749</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>7587768</v>
       </c>
     </row>
@@ -614,73 +624,78 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>C13-label-1</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.5301065</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1.355889</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>179.0559</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>611204.2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>24258.89</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>371972.2</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>439559.7</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>637827.2</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>531790.6</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>1869780</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>2655453</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>724320.4</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>384275.5</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>571942.6</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>1090390</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>128076.8</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>502087.8</v>
       </c>
     </row>
@@ -705,73 +720,78 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>C13-label-2</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.5381745999999999</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1.685469</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>179.0559</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>25542.77</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>17477.71</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>17361.78</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>25262.52</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>30938.68</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>86090.67999999999</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>125686.8</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>36761.19</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>19086.75</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>26148.72</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>57393.56</v>
       </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
       <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
         <v>28516.01</v>
       </c>
     </row>
@@ -796,73 +816,78 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>C13-label-3</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.5398836</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.508562</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>179.0559</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>16745.17</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>7234.489</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
       <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>8311.017</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>11510.11</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>42216.45</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>65303.59</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>13924.05</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>11479.33</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>12266.75</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>16642.14</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>3579.281</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>11868.3</v>
       </c>
     </row>
@@ -887,39 +912,41 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>C13-label-4</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.5580702</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1.500294</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>179.0559</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1152.791</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
       <c r="Q6">
         <v>0</v>
       </c>
@@ -945,15 +972,18 @@
         <v>0</v>
       </c>
       <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
         <v>1457.703</v>
       </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
         <v>0</v>
       </c>
     </row>
@@ -978,36 +1008,38 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>C13-label-5</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.5574932</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2.238175</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>179.0559</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
       <c r="P7">
         <v>0</v>
       </c>
@@ -1018,14 +1050,14 @@
         <v>0</v>
       </c>
       <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>5774.379</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>1457.645</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
       <c r="V7">
         <v>0</v>
       </c>
@@ -1045,6 +1077,9 @@
         <v>0</v>
       </c>
       <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
         <v>0</v>
       </c>
     </row>
@@ -1069,36 +1104,38 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>C13-label-6</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>C6H12O6</t>
         </is>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0.5616493</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0.4946758</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>179.0559</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
       <c r="P8">
         <v>0</v>
       </c>
@@ -1106,11 +1143,11 @@
         <v>0</v>
       </c>
       <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
         <v>1011.62</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
       <c r="T8">
         <v>0</v>
       </c>
@@ -1124,18 +1161,21 @@
         <v>0</v>
       </c>
       <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
         <v>1989.215</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>2921.541</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>1777.58</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>3177.901</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>0</v>
       </c>
     </row>
@@ -1160,73 +1200,78 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>C12 PARENT</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>C3H6O3</t>
         </is>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.8606806</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1.1998</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>89.02428999999999</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>72700000</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>137000000</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>134000000</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>170000000</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>16900000</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>232000000</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>109000000</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>31700000</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>93100000</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>37500000</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>194000000</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>79600000</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>102000000</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>39200000</v>
       </c>
     </row>
@@ -1251,73 +1296,78 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>C13-label-1</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>C3H6O3</t>
         </is>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.8606825</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1.949133</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>89.02428999999999</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>2496721</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>4857564</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>4689536</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>5873392</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>574400.2</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>8085588</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>3883951</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>1122867</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>3234166</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>1277735</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>6889790</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>2808709</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>3560742</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>1390976</v>
       </c>
     </row>
@@ -1342,73 +1392,78 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>C13-label-2</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>C3H6O3</t>
         </is>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.8590307</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2.514325</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>89.02428999999999</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>55478.15</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>119442.5</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>138584.8</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>103296.5</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>14881.87</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>114740.5</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>96995.45</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>23019.65</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>74682.91</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>27564.71</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>104246.1</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>59661.53</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>71813.67999999999</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>29731.18</v>
       </c>
     </row>
@@ -1433,73 +1488,78 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>C13-label-3</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>lactate</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>C3H6O3</t>
         </is>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.8464469999999999</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>1.492148</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>89.02428999999999</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>121073.5</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>102461.1</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>119347.2</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>169835</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>53819.48</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>97697.35000000001</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>109309.9</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>83023.74000000001</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>75536.72</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>66511.00999999999</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>154776.4</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>81949.24000000001</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>150435.8</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>62274.9</v>
       </c>
     </row>
@@ -1510,7 +1570,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1529,70 +1589,75 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>adductName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>BAT-xz971</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Br-xz971</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dia-xz971</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>gas-xz971</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>gWAT-xz971</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>H-xz971</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Kid-xz971</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Liv-xz971</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Lu-xz971</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Pc-xz971</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Q-xz971</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>SI-xz971</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Sol-xz971</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Sp-xz971</t>
         </is>
@@ -1607,46 +1672,51 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D2">
         <v>9553199.890890511</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>481379.86936945</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>6352156.80617231</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>7311072.86675868</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>10836076.4698844</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>8844540.094921321</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>28612722.4768523</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>40317702.5863575</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>11705516.2980777</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>6646281.04684818</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>9169550.941790121</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>16907675.4611845</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>2537065.36340793</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>8223461.12954158</v>
       </c>
     </row>
@@ -1659,12 +1729,14 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D3">
         <v>20483.7859878915</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
         <v>0</v>
       </c>
@@ -1678,27 +1750,30 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>103580.686176551</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>168375.15975918</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>3678.48804379738</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>45362.039738888</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>0</v>
       </c>
     </row>
@@ -1711,46 +1786,51 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D4">
         <v>7796.52408420879</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>6139.25245298429</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4548.2422476682</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>5748.49218415035</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>15947.4322663587</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>31611.6227309111</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>47831.837990903</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>17062.5625690976</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>7056.08051566632</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>10273.7308253397</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>26900.7166866422</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>14684.2760272978</v>
       </c>
     </row>
@@ -1763,46 +1843,51 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D5">
         <v>17014.4015267969</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>7089.49264781115</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>7942.90774143236</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>11076.4819652741</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>41976.3086653958</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>65245.0274485905</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>13429.7036676215</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>11608.2757786005</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>12093.5619426816</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>15492.6598167984</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>3527.32708542237</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>11564.9639029625</v>
       </c>
     </row>
@@ -1815,12 +1900,14 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D6">
         <v>618.081651788915</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
@@ -1846,15 +1933,18 @@
         <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>1108.49326287298</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>0</v>
       </c>
     </row>
@@ -1867,8 +1957,10 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1880,14 +1972,14 @@
         <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>6191.55863568415</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1540.28639733884</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
@@ -1907,6 +1999,9 @@
         <v>0</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>0</v>
       </c>
     </row>
@@ -1919,8 +2014,10 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1929,11 +2026,11 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>1086.84542782207</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>0</v>
       </c>
@@ -1947,18 +2044,21 @@
         <v>0</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>2135.9480285498</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>3136.57467784508</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>1907.72300355334</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>3414.35106837923</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0</v>
       </c>
     </row>
@@ -1971,46 +2071,51 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D9">
         <v>75685330.61167359</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>142624139.9382</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>139501627.427355</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>176980460.063839</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>17594038.9831804</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>241525542.513544</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>113474481.338893</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>33001363.0911662</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>96922646.97425701</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>39039993.7441587</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>201963987.312867</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>82867889.380172</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>106187895.049792</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>40809231.2833188</v>
       </c>
     </row>
@@ -2023,46 +2128,51 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D10">
         <v>142847.401973301</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>427667.93277109</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>353682.986327695</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>371095.427119155</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>26935.8476132564</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>579936.475934481</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>360185.192629893</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>97916.50512002459</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>221186.201212467</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>63173.8981011427</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>618607.716943549</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>234495.301271182</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>260672.171381086</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>123590.239622787</v>
       </c>
     </row>
@@ -2075,46 +2185,51 @@
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D11">
         <v>24301.3350956313</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>61771.426642916</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>83836.3996069319</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>32078.0941085195</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>7048.36593148607</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>19101.7292735674</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>49892.2867246034</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>7667.15432067153</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>36552.201097079</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>11542.2164957695</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>19434.4853030242</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>25372.5640713917</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>27137.3056438291</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>12000.7686052836</v>
       </c>
     </row>
@@ -2127,46 +2242,51 @@
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D12">
         <v>125043.609381403</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>104907.109575394</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>122231.378898289</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>175015.921247931</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>55717.48037392</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>99858.5459914238</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>112316.621861284</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>85947.4531847949</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>77493.37016613589</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>68727.2582627596</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>159347.12588896</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>84349.67628517</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>155325.163880886</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>64306.1337856261</v>
       </c>
     </row>
@@ -2177,7 +2297,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2196,70 +2316,75 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>adductName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>BAT-xz971</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Br-xz971</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Dia-xz971</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>gas-xz971</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>gWAT-xz971</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>H-xz971</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Kid-xz971</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Liv-xz971</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Lu-xz971</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Pc-xz971</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Q-xz971</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>SI-xz971</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Sol-xz971</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Sp-xz971</t>
         </is>
@@ -2274,46 +2399,51 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D2">
         <v>0.995216975280795</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.997921768446822</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.999229832909748</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.998168475233136</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.996780810900273</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.993846151866578</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.993067539758117</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.997401819701339</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.996880148414694</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.996707459819181</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.994724871854726</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.997271360479592</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.9968181622439261</v>
       </c>
     </row>
@@ -2326,12 +2456,14 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D3">
         <v>0.00213392494305573</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
         <v>0</v>
       </c>
@@ -2345,27 +2477,30 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0.00359781444941304</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.0041472577783985</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>0.000399842532898645</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.00266877308296602</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>0</v>
       </c>
     </row>
@@ -2378,46 +2513,51 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D4">
         <v>0.000812212997258541</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>0.000964474563800209</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.000621624134240839</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.0005295241035156839</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.00179727767590381</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.00109801119522235</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.00117814862029881</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.0014538641886288</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.00105834624538172</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.00111672907635227</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.00158264286656977</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>0.00177997473482671</v>
       </c>
     </row>
@@ -2430,46 +2570,51 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D5">
         <v>0.00177249732206046</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>0.00111375698937721</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>0.000731663359078119</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.00124832094792673</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.00145802248878684</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.00160705384318567</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.00114431611003226</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.00174113306365486</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.00131454020819289</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.000911475624566667</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.00138652410460979</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.00140186302124725</v>
       </c>
     </row>
@@ -2482,12 +2627,14 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D6">
         <v>6.43894568307397e-05</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
@@ -2513,15 +2660,18 @@
         <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>0.000120490470174444</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>0</v>
       </c>
     </row>
@@ -2534,8 +2684,10 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2547,14 +2699,14 @@
         <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0.000570337304269994</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.000173590475895935</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
@@ -2574,6 +2726,9 @@
         <v>0</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>0</v>
       </c>
     </row>
@@ -2586,8 +2741,10 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2596,11 +2753,11 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>0.000148542956011167</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>0</v>
       </c>
@@ -2614,18 +2771,21 @@
         <v>0</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>0.000320372276269682</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0.000340937893200451</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0.000112236571171503</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.00134211541579822</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0</v>
       </c>
     </row>
@@ -2638,46 +2798,51 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D9">
         <v>0.996154226472856</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.995850071566183</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.996003532365183</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.996743670645822</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.994927448012465</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.997114672849193</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.995417470003463</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.99422975557812</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.996553165904958</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.996339183506764</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0.996067350984959</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.995863371877469</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.995844224310773</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>0.995125545221531</v>
       </c>
     </row>
@@ -2690,46 +2855,51 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D10">
         <v>0.00188012712722989</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.00298612241687274</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.00252519995799542</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.00208998788935911</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.001523198519199</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.00239421124348493</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.00315960583339959</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.00294992369507928</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.00227422399154369</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.00161226024946404</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.00305091495822116</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.00281804307024161</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.00244461834549674</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>0.00301372509898167</v>
       </c>
     </row>
@@ -2742,46 +2912,51 @@
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D11">
         <v>0.000319849004672413</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.000431309031344541</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.000598569003739874</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.000180661962668165</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.000398578901386736</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>7.885962841548719e-05</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.000437663633603851</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.000230987821477637</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0.00037582766114264</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.000294568760297866</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>9.58490498781421e-05</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.000304914332901535</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.000254497267095196</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>0.000292636519382118</v>
       </c>
     </row>
@@ -2794,46 +2969,51 @@
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="D12">
         <v>0.00164579739524178</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.000732496985599536</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.000872698673081502</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.0009856795021506799</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.00315077456694871</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.000412256278906199</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.000985260529533483</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.00258933290532336</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.000796782442355491</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.00175398748347448</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>0.000785885006941389</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.0010136707193875</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.00145666007663468</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>0.00156809316010487</v>
       </c>
     </row>
@@ -2844,7 +3024,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2858,70 +3038,75 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>adductName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>BAT-xz971</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Br-xz971</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Dia-xz971</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>gas-xz971</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>gWAT-xz971</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>H-xz971</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Kid-xz971</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Liv-xz971</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Lu-xz971</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Pc-xz971</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Q-xz971</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>SI-xz971</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Sol-xz971</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Sp-xz971</t>
         </is>
@@ -2933,46 +3118,51 @@
           <t>glucose</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="C2">
         <v>9599112.684141191</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>481379.86936945</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>6365385.55127311</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>7316707.95443417</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10855959.4284457</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>8873104.29555029</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>28789891.0944252</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>40599154.6115562</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>11736008.5643144</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>6667081.351171</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>9199841.79054266</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>16997338.6004304</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>2544007.04156173</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>8249710.36947184</v>
       </c>
     </row>
@@ -2982,46 +3172,51 @@
           <t>lactate</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>[M-H]-</t>
+        </is>
+      </c>
+      <c r="C3">
         <v>75977522.958124</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>143218486.407189</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>140061378.192188</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>177558649.506314</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>17683740.6770991</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>242224439.264744</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>113996875.440108</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>33192894.2037917</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>97257878.7467327</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>39183437.1170184</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>202761376.641002</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>83212106.9217997</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>106631029.690697</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>41009128.4253325</v>
       </c>
     </row>

</xml_diff>